<commit_message>
added new fuckin files
</commit_message>
<xml_diff>
--- a/CertificationExam3-master/CollectWorkItems/Data/Result.xlsx
+++ b/CertificationExam3-master/CollectWorkItems/Data/Result.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>WIID</t>
   </si>
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -457,176 +457,6 @@
         <v>43536</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>802782</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1">
-        <v>43150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>636492</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1">
-        <v>43516</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>697552</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1">
-        <v>43231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>191382</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1">
-        <v>43141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>479542</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1">
-        <v>43279</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>758992</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="1">
-        <v>43181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>746282</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="1">
-        <v>43188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>583912</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="1">
-        <v>43442</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>367012</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="1">
-        <v>43319</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>419692</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="1">
-        <v>43455</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>